<commit_message>
Plotted force sensor data on second axis
</commit_message>
<xml_diff>
--- a/actuator_python/Data/Jan_7_tests.xlsx
+++ b/actuator_python/Data/Jan_7_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jim/Desktop/Code/Python/P21321/actuator_python/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABCA8BD9-4C1F-AC4A-B6FA-4D2CBF33BE96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4968856-058B-904C-A218-C1BBCA6011B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="5" xr2:uid="{A8662E64-9F95-614A-B36D-193B40FF4537}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{A8662E64-9F95-614A-B36D-193B40FF4537}"/>
   </bookViews>
   <sheets>
     <sheet name="Bottom out 1" sheetId="2" r:id="rId1"/>
@@ -21,14 +21,6 @@
     <sheet name="Test 4" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Test 4'!$B$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Test 4'!$B$2:$B$689</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Test 4'!$C$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Test 4'!$C$2:$C$689</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Test 4'!$B$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Test 4'!$B$2:$B$689</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Test 4'!$C$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Test 4'!$C$2:$C$689</definedName>
     <definedName name="test_01_07_2021__10_41_41" localSheetId="0">'Bottom out 1'!$A$1:$C$699</definedName>
     <definedName name="test_01_07_2021__10_46_53" localSheetId="1">'Bottom out 2'!$A$1:$C$601</definedName>
     <definedName name="test_01_07_2021__10_59_44" localSheetId="2">'Test 1'!$A$1:$C$850</definedName>
@@ -57,7 +49,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{177A0F0F-3592-D647-8DFC-88FB28ECC3D9}" name="test_01_07_2021__10_41_41" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/jim/Desktop/Code/Python/P21321/actuator_python/Data/test_01_07_2021__10_41_41.csv" comma="1">
+    <textPr sourceFile="/Users/jim/Desktop/Code/Python/P21321/actuator_python/Data/test_01_07_2021__10_41_41.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -66,7 +58,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{11E95390-7BA3-644B-85D1-5FAC920E1D7D}" name="test_01_07_2021__10_46_53" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/jim/Desktop/Code/Python/P21321/actuator_python/Data/test_01_07_2021__10_46_53.csv" comma="1">
+    <textPr sourceFile="/Users/jim/Desktop/Code/Python/P21321/actuator_python/Data/test_01_07_2021__10_46_53.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -75,7 +67,7 @@
     </textPr>
   </connection>
   <connection id="3" xr16:uid="{DBFBDF09-81B7-4D49-90AE-274B8C8301C5}" name="test_01_07_2021__10_59_44" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/jim/Desktop/Code/Python/P21321/actuator_python/Data/test_01_07_2021__10_59_44.csv" comma="1">
+    <textPr sourceFile="/Users/jim/Desktop/Code/Python/P21321/actuator_python/Data/test_01_07_2021__10_59_44.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -84,7 +76,7 @@
     </textPr>
   </connection>
   <connection id="4" xr16:uid="{EE0AA7E0-EE86-AA42-A7C1-770402C0716C}" name="test_drill_test_2_jan_7" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/jim/Desktop/Code/Python/P21321/actuator_python/Data/test_drill_test_2_jan_7.csv" comma="1">
+    <textPr sourceFile="/Users/jim/Desktop/Code/Python/P21321/actuator_python/Data/test_drill_test_2_jan_7.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -93,7 +85,7 @@
     </textPr>
   </connection>
   <connection id="5" xr16:uid="{0865A63F-9022-4F48-B464-C998DE5DDB77}" name="test_drill_test_3_jan_7" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/jim/Desktop/Code/Python/P21321/actuator_python/Data/test_drill_test_3_jan_7.csv" comma="1">
+    <textPr sourceFile="/Users/jim/Desktop/Code/Python/P21321/actuator_python/Data/test_drill_test_3_jan_7.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -102,7 +94,7 @@
     </textPr>
   </connection>
   <connection id="6" xr16:uid="{90538A14-344D-8240-90FA-3E5B9584ADC7}" name="test_drill_test_4_jan_7" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/jim/Desktop/Code/Python/P21321/actuator_python/Data/test_drill_test_4_jan_7.csv" comma="1">
+    <textPr sourceFile="/Users/jim/Desktop/Code/Python/P21321/actuator_python/Data/test_drill_test_4_jan_7.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -2363,6 +2355,22 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1167769983"/>
+        <c:axId val="1167390719"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -4507,9 +4515,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1167769983"/>
-        <c:axId val="1167390719"/>
+        <c:axId val="818046207"/>
+        <c:axId val="816366383"/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="1167769983"/>
@@ -4618,6 +4627,64 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="816366383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="818046207"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="818046207"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="816366383"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -6586,6 +6653,22 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1169127151"/>
+        <c:axId val="1134825103"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -8436,9 +8519,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1169127151"/>
-        <c:axId val="1134825103"/>
+        <c:axId val="817166479"/>
+        <c:axId val="817679279"/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="1169127151"/>
@@ -8547,6 +8631,64 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="817679279"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="817166479"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="817166479"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="817679279"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -11262,6 +11404,22 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1169769439"/>
+        <c:axId val="1169771087"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -13859,9 +14017,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1169769439"/>
-        <c:axId val="1169771087"/>
+        <c:axId val="814058447"/>
+        <c:axId val="787048543"/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="1169769439"/>
@@ -13970,6 +14129,64 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="787048543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="814058447"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="814058447"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="787048543"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -16457,6 +16674,22 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1167620175"/>
+        <c:axId val="1167879439"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -18826,9 +19059,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1167620175"/>
-        <c:axId val="1167879439"/>
+        <c:axId val="785251311"/>
+        <c:axId val="814315743"/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="1167620175"/>
@@ -18937,6 +19171,64 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="814315743"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="785251311"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="785251311"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="814315743"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -21196,6 +21488,22 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1170190943"/>
+        <c:axId val="1169272351"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -23337,9 +23645,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1170190943"/>
-        <c:axId val="1169272351"/>
+        <c:axId val="785350991"/>
+        <c:axId val="784682687"/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="1170190943"/>
@@ -23448,6 +23757,64 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="784682687"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="785350991"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="785350991"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="784682687"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -25680,6 +26047,22 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1176461903"/>
+        <c:axId val="1176463551"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -27794,9 +28177,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1176461903"/>
-        <c:axId val="1176463551"/>
+        <c:axId val="786677327"/>
+        <c:axId val="785142271"/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="1176461903"/>
@@ -27905,6 +28289,64 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="785142271"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="786677327"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="786677327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="785142271"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -31886,8 +32328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7A1751-6C5E-2F4D-95EF-C73CCAE67FC7}">
   <dimension ref="A1:C699"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -71833,8 +72275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A61EB1-3B72-1E4D-89F5-0CD63E7CC033}">
   <dimension ref="A1:C689"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>